<commit_message>
1. modify JinMeiYouKanJi 2. add ByakuYaKou
</commit_message>
<xml_diff>
--- a/人名用漢字.xlsx
+++ b/人名用漢字.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8520" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8520"/>
   </bookViews>
   <sheets>
     <sheet name="漢字読み方あかさたな" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="263">
   <si>
     <t>あ</t>
   </si>
@@ -795,6 +795,18 @@
   </si>
   <si>
     <t>憲</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ささ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>笹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>垣</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -854,7 +866,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -865,6 +877,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1165,9 +1180,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:U22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U11" sqref="U11"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.625" defaultRowHeight="13.5"/>
@@ -1294,6 +1309,9 @@
       <c r="H4" t="s">
         <v>29</v>
       </c>
+      <c r="I4" t="s">
+        <v>262</v>
+      </c>
       <c r="K4" s="1" t="s">
         <v>30</v>
       </c>
@@ -1371,13 +1389,10 @@
         <v>53</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L6" t="s">
-        <v>55</v>
-      </c>
-      <c r="M6" t="s">
-        <v>56</v>
+        <v>260</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>261</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>57</v>
@@ -1409,10 +1424,13 @@
         <v>65</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="L7" t="s">
-        <v>67</v>
+        <v>55</v>
+      </c>
+      <c r="M7" t="s">
+        <v>56</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>68</v>
@@ -1450,10 +1468,10 @@
         <v>78</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="L8" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>81</v>
@@ -1482,10 +1500,10 @@
         <v>88</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="L9" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>91</v>
@@ -1514,10 +1532,10 @@
         <v>98</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="L10" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>101</v>
@@ -1555,16 +1573,10 @@
         <v>110</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="L11" t="s">
-        <v>112</v>
-      </c>
-      <c r="M11" t="s">
-        <v>113</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>114</v>
@@ -1587,10 +1599,16 @@
         <v>119</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="L12" t="s">
-        <v>121</v>
+        <v>112</v>
+      </c>
+      <c r="M12" t="s">
+        <v>113</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>122</v>
@@ -1613,10 +1631,10 @@
         <v>127</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="L13" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>130</v>
@@ -1648,10 +1666,10 @@
         <v>138</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="L14" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>141</v>
@@ -1674,10 +1692,10 @@
         <v>146</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="L15" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>149</v>
@@ -1703,10 +1721,10 @@
         <v>155</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="L16" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>163</v>
@@ -1729,13 +1747,10 @@
         <v>168</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L17" t="s">
-        <v>161</v>
-      </c>
-      <c r="M17" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="O17" s="1" t="s">
         <v>171</v>
@@ -1761,10 +1776,13 @@
         <v>176</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="L18" t="s">
-        <v>170</v>
+        <v>161</v>
+      </c>
+      <c r="M18" t="s">
+        <v>162</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>177</v>
@@ -1779,6 +1797,12 @@
       </c>
       <c r="C19" t="s">
         <v>174</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="L19" t="s">
+        <v>170</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>179</v>
@@ -1821,7 +1845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:V13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>

</xml_diff>